<commit_message>
change all units to SI/pint-compatible
</commit_message>
<xml_diff>
--- a/tests/data/test_RCP_database_raw_download.xlsx
+++ b/tests/data/test_RCP_database_raw_download.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/Github/pyam/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156B79FC-21FB-CC44-B4AC-C35EAAF6BF14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA52316D-3A60-1E42-A155-AB5675F55940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>Primary Energy</t>
   </si>
   <si>
-    <t>EJ/y</t>
-  </si>
-  <si>
     <t>1) Note that RCP 6.0 concentration data are not harmonized to the same base year across the models yet. Harmonized data is under preparation and will be added soon.</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>model_a - scen_a</t>
+  </si>
+  <si>
+    <t>EJ</t>
   </si>
 </sst>
 </file>
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -503,7 +503,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -512,7 +512,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -521,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -535,16 +535,16 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3">
         <v>0.5</v>
@@ -553,7 +553,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -567,7 +567,7 @@
     </row>
     <row r="4" spans="1:17" ht="250.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>

</xml_diff>

<commit_message>
switching back to `EJ/yr` as requested by @gidden
</commit_message>
<xml_diff>
--- a/tests/data/test_RCP_database_raw_download.xlsx
+++ b/tests/data/test_RCP_database_raw_download.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/Github/pyam/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA52316D-3A60-1E42-A155-AB5675F55940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E12201-2513-7446-911B-79F68EF718E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
     <t>model_a - scen_a</t>
   </si>
   <si>
-    <t>EJ</t>
+    <t>EJ/yr</t>
   </si>
 </sst>
 </file>
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
use `pint` and iamc-units repo for unit conversion (#341)
</commit_message>
<xml_diff>
--- a/tests/data/test_RCP_database_raw_download.xlsx
+++ b/tests/data/test_RCP_database_raw_download.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/Github/pyam/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156B79FC-21FB-CC44-B4AC-C35EAAF6BF14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E12201-2513-7446-911B-79F68EF718E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>Primary Energy</t>
   </si>
   <si>
-    <t>EJ/y</t>
-  </si>
-  <si>
     <t>1) Note that RCP 6.0 concentration data are not harmonized to the same base year across the models yet. Harmonized data is under preparation and will be added soon.</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>model_a - scen_a</t>
+  </si>
+  <si>
+    <t>EJ/yr</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -503,7 +503,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -512,7 +512,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -521,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -535,16 +535,16 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3">
         <v>0.5</v>
@@ -553,7 +553,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -567,7 +567,7 @@
     </row>
     <row r="4" spans="1:17" ht="250.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>

</xml_diff>